<commit_message>
fixed the transposing parsing syntax error
</commit_message>
<xml_diff>
--- a/data/costs.xlsx
+++ b/data/costs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Myles\OneDrive\Desktop\Dasboard.Alpha\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8468D2D9-3450-4C24-A3CB-CB496ED04D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF677CA-9442-43CD-9F59-BED7C30A331E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3000" yWindow="732" windowWidth="17280" windowHeight="9960" xr2:uid="{F8EAEC73-6452-431E-B126-AB3351F256CB}"/>
+    <workbookView xWindow="0" yWindow="732" windowWidth="17280" windowHeight="9960" xr2:uid="{F8EAEC73-6452-431E-B126-AB3351F256CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -471,6 +471,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="14.21875" customWidth="1"/>
     <col min="2" max="8" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>